<commit_message>
Update Packet Rate Calculations
</commit_message>
<xml_diff>
--- a/doc/PRooFPS-dd-Packet-Rates.xlsx
+++ b/doc/PRooFPS-dd-Packet-Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PGE\PGE\docpages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PRooFPS-dd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F55768-2F80-45F8-A186-71811D254363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2747C66E-23B8-4E82-817F-7AE319A19374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Sizes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="93">
   <si>
     <t>v0.1.2</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>Momentary aim accuracy added to UserUpdateFromServer.</t>
+  </si>
+  <si>
+    <t>v0.3.0</t>
+  </si>
+  <si>
+    <t>WeaponId in BulletUpdateFromServer.</t>
   </si>
 </sst>
 </file>
@@ -1247,6 +1253,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1289,9 +1337,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,45 +1348,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1692,11 +1698,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECDFA06-7C74-467D-91F0-6C7F3FAEFF70}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="11" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,15 +2324,37 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="69"/>
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="41">
+        <f>16+15</f>
+        <v>31</v>
+      </c>
+      <c r="D28" s="56">
+        <f>60+15</f>
+        <v>75</v>
+      </c>
+      <c r="E28" s="10">
+        <f>8+15</f>
+        <v>23</v>
+      </c>
+      <c r="F28" s="10">
+        <f>88+15</f>
+        <v>103</v>
+      </c>
+      <c r="G28" s="10">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
+      <c r="H28" s="69">
+        <f>52+15</f>
+        <v>67</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -2548,10 +2576,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C73525B-4602-4ED0-8F77-5C69A22A2F34}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="R43" sqref="R43"/>
+      <selection pane="topRight" activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2729,87 +2757,87 @@
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="88" t="s">
+      <c r="D27" s="101"/>
+      <c r="E27" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="85" t="s">
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="86"/>
-      <c r="P27" s="86"/>
-      <c r="Q27" s="87"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="101"/>
     </row>
     <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="98" t="s">
+      <c r="A28" s="92"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="100" t="s">
+      <c r="E28" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91" t="s">
+      <c r="F28" s="82"/>
+      <c r="G28" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="93" t="s">
+      <c r="H28" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="91" t="s">
+      <c r="I28" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="91" t="s">
+      <c r="J28" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="95"/>
-      <c r="L28" s="101" t="s">
+      <c r="K28" s="108"/>
+      <c r="L28" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="102"/>
-      <c r="N28" s="89" t="s">
+      <c r="M28" s="84"/>
+      <c r="N28" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="90"/>
-      <c r="P28" s="83" t="s">
+      <c r="O28" s="104"/>
+      <c r="P28" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="Q28" s="84"/>
+      <c r="Q28" s="98"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="104"/>
+      <c r="A29" s="93"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="86"/>
       <c r="E29" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="92"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="92"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="107"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="19" t="s">
         <v>65</v>
       </c>
@@ -2850,11 +2878,11 @@
         <f>1-(C30/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="108">
+      <c r="E30" s="90">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="F30" s="105"/>
+      <c r="F30" s="87"/>
       <c r="G30" s="7">
         <f>$C$10*$C$13</f>
         <v>480</v>
@@ -2867,11 +2895,11 @@
         <f>$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J30" s="105">
+      <c r="J30" s="87">
         <f>$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K30" s="106"/>
+      <c r="K30" s="88"/>
       <c r="L30" s="22">
         <f t="shared" ref="L30:L45" si="0">E30+G30+H30+I30+J30</f>
         <v>4327</v>
@@ -2915,14 +2943,14 @@
         <v>480</v>
       </c>
       <c r="D31" s="58">
-        <f t="shared" ref="D31:D44" si="2">1-(C31/$C$30)</f>
+        <f t="shared" ref="D31:D43" si="2">1-(C31/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="96">
+      <c r="E31" s="77">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F31" s="97"/>
+      <c r="F31" s="78"/>
       <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2935,11 +2963,11 @@
         <f t="shared" ref="I31:I33" si="4">$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J31" s="97">
+      <c r="J31" s="78">
         <f t="shared" ref="J31:J32" si="5">$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K31" s="107"/>
+      <c r="K31" s="89"/>
       <c r="L31" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -2953,15 +2981,15 @@
         <v>30289</v>
       </c>
       <c r="O31" s="11">
-        <f t="shared" ref="O31:O45" si="7">7*M31</f>
+        <f t="shared" ref="O31:O46" si="7">7*M31</f>
         <v>30289</v>
       </c>
       <c r="P31" s="53">
-        <f t="shared" ref="P31:P45" si="8">1-(N31/$N$30)</f>
+        <f t="shared" ref="P31:P46" si="8">1-(N31/$N$30)</f>
         <v>0</v>
       </c>
       <c r="Q31" s="54">
-        <f t="shared" ref="Q31:Q45" si="9">1-(O31/$O$30)</f>
+        <f t="shared" ref="Q31:Q46" si="9">1-(O31/$O$30)</f>
         <v>0</v>
       </c>
       <c r="R31" s="4"/>
@@ -2986,11 +3014,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E32" s="96">
+      <c r="E32" s="77">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F32" s="97"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -3003,11 +3031,11 @@
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J32" s="97">
+      <c r="J32" s="78">
         <f t="shared" si="5"/>
         <v>2880</v>
       </c>
-      <c r="K32" s="107"/>
+      <c r="K32" s="89"/>
       <c r="L32" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -3054,11 +3082,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="96">
+      <c r="E33" s="77">
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F33" s="97"/>
+      <c r="F33" s="78"/>
       <c r="G33" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3125,11 +3153,11 @@
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
-      <c r="E34" s="96">
+      <c r="E34" s="77">
         <f t="shared" ref="E34" si="10">$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F34" s="97"/>
+      <c r="F34" s="78"/>
       <c r="G34" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3189,7 +3217,7 @@
         <v>63</v>
       </c>
       <c r="C35" s="41">
-        <f t="shared" ref="C35:C45" si="11">16*$C$10</f>
+        <f t="shared" ref="C35:C46" si="11">16*$C$10</f>
         <v>128</v>
       </c>
       <c r="D35" s="58">
@@ -3201,7 +3229,7 @@
         <v>160</v>
       </c>
       <c r="F35" s="10">
-        <f t="shared" ref="F35:F45" si="12">$C$10*$C$16</f>
+        <f t="shared" ref="F35:F46" si="12">$C$10*$C$16</f>
         <v>480</v>
       </c>
       <c r="G35" s="10">
@@ -3217,11 +3245,11 @@
         <v>14</v>
       </c>
       <c r="J35" s="10">
-        <f t="shared" ref="J35:J45" si="14">$C$10*$C$15</f>
+        <f t="shared" ref="J35:J46" si="14">$C$10*$C$15</f>
         <v>160</v>
       </c>
       <c r="K35" s="21">
-        <f t="shared" ref="K35:K45" si="15">$C$10*$C$14</f>
+        <f t="shared" ref="K35:K46" si="15">$C$10*$C$14</f>
         <v>480</v>
       </c>
       <c r="L35" s="23">
@@ -3229,7 +3257,7 @@
         <v>881</v>
       </c>
       <c r="M35" s="11">
-        <f t="shared" ref="M35:M45" si="16">F35+G35+H35+I35+K35</f>
+        <f t="shared" ref="M35:M46" si="16">F35+G35+H35+I35+K35</f>
         <v>1521</v>
       </c>
       <c r="N35" s="23">
@@ -3271,7 +3299,7 @@
         <v>0.73333333333333339</v>
       </c>
       <c r="E36" s="9">
-        <f t="shared" ref="E36:E45" si="17">$C$10*$C$17</f>
+        <f t="shared" ref="E36:E46" si="17">$C$10*$C$17</f>
         <v>160</v>
       </c>
       <c r="F36" s="10">
@@ -3279,11 +3307,11 @@
         <v>480</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" ref="G36:G45" si="18">$C$10*$C$14</f>
+        <f t="shared" ref="G36:G46" si="18">$C$10*$C$14</f>
         <v>480</v>
       </c>
       <c r="H36" s="21">
-        <f t="shared" ref="H36:H45" si="19">7 + 1*$C$13</f>
+        <f t="shared" ref="H36:H46" si="19">7 + 1*$C$13</f>
         <v>67</v>
       </c>
       <c r="I36" s="10">
@@ -3657,7 +3685,7 @@
         <v>67</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" ref="I41:I45" si="20">$C$9*2 + $C$9*2</f>
+        <f t="shared" ref="I41:I46" si="20">$C$9*2 + $C$9*2</f>
         <v>28</v>
       </c>
       <c r="J41" s="10">
@@ -3965,7 +3993,7 @@
         <v>480</v>
       </c>
       <c r="L45" s="23">
-        <f t="shared" si="0"/>
+        <f>E45+G45+H45+I45+J45</f>
         <v>895</v>
       </c>
       <c r="M45" s="11">
@@ -3973,7 +4001,7 @@
         <v>1535</v>
       </c>
       <c r="N45" s="23">
-        <f t="shared" si="6"/>
+        <f>7*L45</f>
         <v>6265</v>
       </c>
       <c r="O45" s="11">
@@ -3996,23 +4024,72 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="54"/>
+      <c r="A46" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="41">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+      <c r="D46" s="58">
+        <f>1-(C46/$C$30)</f>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" si="17"/>
+        <v>160</v>
+      </c>
+      <c r="F46" s="10">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="G46" s="10">
+        <f t="shared" si="18"/>
+        <v>480</v>
+      </c>
+      <c r="H46" s="21">
+        <f t="shared" si="19"/>
+        <v>67</v>
+      </c>
+      <c r="I46" s="10">
+        <f t="shared" si="20"/>
+        <v>28</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="14"/>
+        <v>160</v>
+      </c>
+      <c r="K46" s="21">
+        <f t="shared" si="15"/>
+        <v>480</v>
+      </c>
+      <c r="L46" s="23">
+        <f>E46+G46+H46+I46+J46</f>
+        <v>895</v>
+      </c>
+      <c r="M46" s="11">
+        <f t="shared" si="16"/>
+        <v>1535</v>
+      </c>
+      <c r="N46" s="23">
+        <f>7*L46</f>
+        <v>6265</v>
+      </c>
+      <c r="O46" s="11">
+        <f t="shared" si="7"/>
+        <v>10745</v>
+      </c>
+      <c r="P46" s="53">
+        <f t="shared" si="8"/>
+        <v>0.79315923272475153</v>
+      </c>
+      <c r="Q46" s="54">
+        <f t="shared" si="9"/>
+        <v>0.64525075109775831</v>
+      </c>
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
@@ -4228,6 +4305,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C28:C29"/>
@@ -4240,17 +4328,6 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D51">
     <cfRule type="colorScale" priority="17">
@@ -4348,7 +4425,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30:O45">
+  <conditionalFormatting sqref="N30:O46">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4360,7 +4437,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P30:Q45">
+  <conditionalFormatting sqref="P30:Q46">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4380,9 +4457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A631036-56BD-4CE5-917C-895C0C771D72}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E35" sqref="E35"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4450,87 +4527,87 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="88" t="s">
+      <c r="D15" s="101"/>
+      <c r="E15" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="85" t="s">
+      <c r="F15" s="102"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="86"/>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="87"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="101"/>
     </row>
     <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="98" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91" t="s">
+      <c r="F16" s="82"/>
+      <c r="G16" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="93" t="s">
+      <c r="H16" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="91" t="s">
+      <c r="J16" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="95"/>
-      <c r="L16" s="101" t="s">
+      <c r="K16" s="108"/>
+      <c r="L16" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="102"/>
-      <c r="N16" s="89" t="s">
+      <c r="M16" s="84"/>
+      <c r="N16" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="90"/>
-      <c r="P16" s="83" t="s">
+      <c r="O16" s="104"/>
+      <c r="P16" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="84"/>
+      <c r="Q16" s="98"/>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="104"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="86"/>
       <c r="E17" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="92"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="92"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="19" t="s">
         <v>65</v>
       </c>
@@ -4588,11 +4665,11 @@
         <f>'Packet Rates'!I30*'Packet Sizes'!G12</f>
         <v>112560</v>
       </c>
-      <c r="J18" s="105">
+      <c r="J18" s="87">
         <f>'Packet Rates'!J30*'Packet Sizes'!H12</f>
         <v>771840</v>
       </c>
-      <c r="K18" s="106"/>
+      <c r="K18" s="88"/>
       <c r="L18" s="22">
         <f>E18+G18+H18+I18+J18</f>
         <v>1159636</v>
@@ -4650,11 +4727,11 @@
         <f>'Packet Rates'!I31*'Packet Sizes'!G13</f>
         <v>112560</v>
       </c>
-      <c r="J19" s="97">
+      <c r="J19" s="78">
         <f>'Packet Rates'!J31*'Packet Sizes'!H13</f>
         <v>771840</v>
       </c>
-      <c r="K19" s="107"/>
+      <c r="K19" s="89"/>
       <c r="L19" s="23">
         <f t="shared" ref="L19:L33" si="1">E19+G19+H19+I19+J19</f>
         <v>1159636</v>
@@ -4712,11 +4789,11 @@
         <f>'Packet Rates'!I32*'Packet Sizes'!G14</f>
         <v>112560</v>
       </c>
-      <c r="J20" s="97">
+      <c r="J20" s="78">
         <f>'Packet Rates'!J32*'Packet Sizes'!H14</f>
         <v>771840</v>
       </c>
-      <c r="K20" s="107"/>
+      <c r="K20" s="89"/>
       <c r="L20" s="23">
         <f t="shared" si="1"/>
         <v>1159636</v>
@@ -4757,11 +4834,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="96">
+      <c r="E21" s="77">
         <f>'Packet Rates'!E33*'Packet Sizes'!D15</f>
         <v>42880</v>
       </c>
-      <c r="F21" s="97"/>
+      <c r="F21" s="78"/>
       <c r="G21" s="10">
         <f>'Packet Rates'!G33*'Packet Sizes'!E15</f>
         <v>42880</v>
@@ -4822,11 +4899,11 @@
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
-      <c r="E22" s="96">
+      <c r="E22" s="77">
         <f>'Packet Rates'!E34*'Packet Sizes'!D16</f>
         <v>8800</v>
       </c>
-      <c r="F22" s="97"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="10">
         <f>'Packet Rates'!G34*'Packet Sizes'!E16</f>
         <v>3680</v>
@@ -5621,23 +5698,72 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="54"/>
+      <c r="A34" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="41">
+        <f>'Packet Rates'!C46*'Packet Sizes'!C28</f>
+        <v>3968</v>
+      </c>
+      <c r="D34" s="61">
+        <f t="shared" ref="D34" si="8">1-(C34/$C$18)</f>
+        <v>0.96915422885572144</v>
+      </c>
+      <c r="E34" s="9">
+        <f>'Packet Rates'!E46*'Packet Sizes'!D28</f>
+        <v>12000</v>
+      </c>
+      <c r="F34" s="10">
+        <f>'Packet Rates'!F46*'Packet Sizes'!D28</f>
+        <v>36000</v>
+      </c>
+      <c r="G34" s="10">
+        <f>'Packet Rates'!G46*'Packet Sizes'!E28</f>
+        <v>11040</v>
+      </c>
+      <c r="H34" s="10">
+        <f>'Packet Rates'!H46*'Packet Sizes'!F28</f>
+        <v>6901</v>
+      </c>
+      <c r="I34" s="10">
+        <f>'Packet Rates'!I46*'Packet Sizes'!G28</f>
+        <v>2324</v>
+      </c>
+      <c r="J34" s="10">
+        <f>'Packet Rates'!J46*'Packet Sizes'!H28</f>
+        <v>10720</v>
+      </c>
+      <c r="K34" s="21">
+        <f>'Packet Rates'!K46*'Packet Sizes'!H28</f>
+        <v>32160</v>
+      </c>
+      <c r="L34" s="23">
+        <f t="shared" ref="L34" si="9">E34+G34+H34+I34+J34</f>
+        <v>42985</v>
+      </c>
+      <c r="M34" s="11">
+        <f t="shared" ref="M34" si="10">F34+G34+H34+I34+K34</f>
+        <v>88425</v>
+      </c>
+      <c r="N34" s="23">
+        <f t="shared" ref="N34" si="11">L34*7</f>
+        <v>300895</v>
+      </c>
+      <c r="O34" s="11">
+        <f t="shared" ref="O34" si="12">M34*7</f>
+        <v>618975</v>
+      </c>
+      <c r="P34" s="53">
+        <f t="shared" ref="P34" si="13">1-(N34/$N$18)</f>
+        <v>0.96293233393927058</v>
+      </c>
+      <c r="Q34" s="54">
+        <f t="shared" ref="Q34" si="14">1-(O34/$O$18)</f>
+        <v>0.9237476242545074</v>
+      </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
@@ -5736,6 +5862,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="E15:M15"/>
@@ -5750,15 +5885,6 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:D39">
     <cfRule type="colorScale" priority="17">
@@ -5868,7 +5994,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P33">
+  <conditionalFormatting sqref="P18:P34">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5932,7 +6058,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18:Q33">
+  <conditionalFormatting sqref="Q18:Q34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Update Pkt Rate Calc for v0.4.2.
</commit_message>
<xml_diff>
--- a/doc/PRooFPS-dd-Packet-Rates.xlsx
+++ b/doc/PRooFPS-dd-Packet-Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PRooFPS-dd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B677D276-D412-4AF5-A302-AACB03A68E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCF81F2-4141-45BE-B7AE-A34D21548E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="94">
   <si>
     <t>v0.1.2</t>
   </si>
@@ -319,10 +319,7 @@
     <t>WeaponId in BulletUpdateFromServer.</t>
   </si>
   <si>
-    <t>v0.4.1</t>
-  </si>
-  <si>
-    <t>v0.4.1.</t>
+    <t>v0.4.2</t>
   </si>
 </sst>
 </file>
@@ -1259,6 +1256,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1301,9 +1340,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1315,45 +1351,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1708,7 +1705,7 @@
       <pane xSplit="1" ySplit="11" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2604,7 @@
     <sheetView topLeftCell="A29" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="R47" sqref="R47"/>
+      <selection pane="topRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,87 +2782,87 @@
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="88" t="s">
+      <c r="D27" s="101"/>
+      <c r="E27" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="85" t="s">
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="86"/>
-      <c r="P27" s="86"/>
-      <c r="Q27" s="87"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="101"/>
     </row>
     <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="98" t="s">
+      <c r="A28" s="92"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="100" t="s">
+      <c r="E28" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91" t="s">
+      <c r="F28" s="82"/>
+      <c r="G28" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="93" t="s">
+      <c r="H28" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="91" t="s">
+      <c r="I28" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="91" t="s">
+      <c r="J28" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="95"/>
-      <c r="L28" s="101" t="s">
+      <c r="K28" s="108"/>
+      <c r="L28" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="102"/>
-      <c r="N28" s="89" t="s">
+      <c r="M28" s="84"/>
+      <c r="N28" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="90"/>
-      <c r="P28" s="83" t="s">
+      <c r="O28" s="104"/>
+      <c r="P28" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="Q28" s="84"/>
+      <c r="Q28" s="98"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="104"/>
+      <c r="A29" s="93"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="86"/>
       <c r="E29" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="92"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="92"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="107"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="19" t="s">
         <v>65</v>
       </c>
@@ -2906,11 +2903,11 @@
         <f>1-(C30/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="108">
+      <c r="E30" s="90">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="F30" s="105"/>
+      <c r="F30" s="87"/>
       <c r="G30" s="7">
         <f>$C$10*$C$13</f>
         <v>480</v>
@@ -2923,11 +2920,11 @@
         <f>$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J30" s="105">
+      <c r="J30" s="87">
         <f>$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K30" s="106"/>
+      <c r="K30" s="88"/>
       <c r="L30" s="22">
         <f t="shared" ref="L30:L44" si="0">E30+G30+H30+I30+J30</f>
         <v>4327</v>
@@ -2974,11 +2971,11 @@
         <f t="shared" ref="D31:D43" si="2">1-(C31/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="96">
+      <c r="E31" s="77">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F31" s="97"/>
+      <c r="F31" s="78"/>
       <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2991,11 +2988,11 @@
         <f t="shared" ref="I31:I33" si="4">$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J31" s="97">
+      <c r="J31" s="78">
         <f t="shared" ref="J31:J32" si="5">$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K31" s="107"/>
+      <c r="K31" s="89"/>
       <c r="L31" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -3042,11 +3039,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E32" s="96">
+      <c r="E32" s="77">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F32" s="97"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -3059,11 +3056,11 @@
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J32" s="97">
+      <c r="J32" s="78">
         <f t="shared" si="5"/>
         <v>2880</v>
       </c>
-      <c r="K32" s="107"/>
+      <c r="K32" s="89"/>
       <c r="L32" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -3110,11 +3107,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="96">
+      <c r="E33" s="77">
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F33" s="97"/>
+      <c r="F33" s="78"/>
       <c r="G33" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3181,11 +3178,11 @@
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
-      <c r="E34" s="96">
+      <c r="E34" s="77">
         <f t="shared" ref="E34" si="10">$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F34" s="97"/>
+      <c r="F34" s="78"/>
       <c r="G34" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -4382,6 +4379,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C28:C29"/>
@@ -4394,17 +4402,6 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D51">
     <cfRule type="colorScale" priority="17">
@@ -4536,7 +4533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R34" sqref="R34"/>
+      <selection pane="topRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,87 +4601,87 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="88" t="s">
+      <c r="D15" s="101"/>
+      <c r="E15" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="85" t="s">
+      <c r="F15" s="102"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="86"/>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="87"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="101"/>
     </row>
     <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="98" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91" t="s">
+      <c r="F16" s="82"/>
+      <c r="G16" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="93" t="s">
+      <c r="H16" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="91" t="s">
+      <c r="J16" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="95"/>
-      <c r="L16" s="101" t="s">
+      <c r="K16" s="108"/>
+      <c r="L16" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="102"/>
-      <c r="N16" s="89" t="s">
+      <c r="M16" s="84"/>
+      <c r="N16" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="90"/>
-      <c r="P16" s="83" t="s">
+      <c r="O16" s="104"/>
+      <c r="P16" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="84"/>
+      <c r="Q16" s="98"/>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="104"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="86"/>
       <c r="E17" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="92"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="92"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="19" t="s">
         <v>65</v>
       </c>
@@ -4742,11 +4739,11 @@
         <f>'Packet Rates'!I30*'Packet Sizes'!G12</f>
         <v>112560</v>
       </c>
-      <c r="J18" s="105">
+      <c r="J18" s="87">
         <f>'Packet Rates'!J30*'Packet Sizes'!H12</f>
         <v>771840</v>
       </c>
-      <c r="K18" s="106"/>
+      <c r="K18" s="88"/>
       <c r="L18" s="22">
         <f>E18+G18+H18+I18+J18</f>
         <v>1159636</v>
@@ -4804,11 +4801,11 @@
         <f>'Packet Rates'!I31*'Packet Sizes'!G13</f>
         <v>112560</v>
       </c>
-      <c r="J19" s="97">
+      <c r="J19" s="78">
         <f>'Packet Rates'!J31*'Packet Sizes'!H13</f>
         <v>771840</v>
       </c>
-      <c r="K19" s="107"/>
+      <c r="K19" s="89"/>
       <c r="L19" s="23">
         <f t="shared" ref="L19:L33" si="1">E19+G19+H19+I19+J19</f>
         <v>1159636</v>
@@ -4866,11 +4863,11 @@
         <f>'Packet Rates'!I32*'Packet Sizes'!G14</f>
         <v>112560</v>
       </c>
-      <c r="J20" s="97">
+      <c r="J20" s="78">
         <f>'Packet Rates'!J32*'Packet Sizes'!H14</f>
         <v>771840</v>
       </c>
-      <c r="K20" s="107"/>
+      <c r="K20" s="89"/>
       <c r="L20" s="23">
         <f t="shared" si="1"/>
         <v>1159636</v>
@@ -4911,11 +4908,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="96">
+      <c r="E21" s="77">
         <f>'Packet Rates'!E33*'Packet Sizes'!D15</f>
         <v>42880</v>
       </c>
-      <c r="F21" s="97"/>
+      <c r="F21" s="78"/>
       <c r="G21" s="10">
         <f>'Packet Rates'!G33*'Packet Sizes'!E15</f>
         <v>42880</v>
@@ -4976,11 +4973,11 @@
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
-      <c r="E22" s="96">
+      <c r="E22" s="77">
         <f>'Packet Rates'!E34*'Packet Sizes'!D16</f>
         <v>8800</v>
       </c>
-      <c r="F22" s="97"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="10">
         <f>'Packet Rates'!G34*'Packet Sizes'!E16</f>
         <v>3680</v>
@@ -5844,7 +5841,7 @@
     </row>
     <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>29</v>
@@ -5988,6 +5985,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="E15:M15"/>
@@ -6002,15 +6008,6 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:D39">
     <cfRule type="colorScale" priority="17">

</xml_diff>

<commit_message>
Update Packet Rates Table
</commit_message>
<xml_diff>
--- a/doc/PRooFPS-dd-Packet-Rates.xlsx
+++ b/doc/PRooFPS-dd-Packet-Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PRooFPS-dd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31334931-41E9-41EB-B19C-286122630854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D946301-4CF1-4F86-87A8-469AF43A6B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Sizes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="108">
   <si>
     <t>v0.1.2</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t>Mch pistol firing rate: ~7 -&gt; 20 bullets / sec.</t>
+  </si>
+  <si>
+    <t>v0.6.0</t>
+  </si>
+  <si>
+    <t>Add toggleItem and currentItemPower to UserCmdFromClient and UserUpdateFromServer.</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1076,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1101,15 +1107,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1128,12 +1125,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1150,25 +1141,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1268,6 +1249,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1310,9 +1336,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,64 +1348,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1722,11 +1703,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECDFA06-7C74-467D-91F0-6C7F3FAEFF70}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,42 +1756,42 @@
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="64"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="55"/>
     </row>
     <row r="11" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="42" t="s">
+      <c r="A11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="2"/>
@@ -1825,28 +1806,28 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="48">
         <v>268</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="49">
         <v>268</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="50">
         <v>268</v>
       </c>
-      <c r="F12" s="59">
+      <c r="F12" s="50">
         <v>268</v>
       </c>
-      <c r="G12" s="59">
+      <c r="G12" s="50">
         <v>268</v>
       </c>
-      <c r="H12" s="60">
+      <c r="H12" s="51">
         <v>268</v>
       </c>
       <c r="I12" s="5"/>
@@ -1857,16 +1838,16 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="26">
         <v>268</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="39">
         <v>268</v>
       </c>
       <c r="E13" s="10">
@@ -1878,7 +1859,7 @@
       <c r="G13" s="10">
         <v>268</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="52">
         <v>268</v>
       </c>
       <c r="I13" s="5"/>
@@ -1889,16 +1870,16 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="26">
         <v>268</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="39">
         <v>268</v>
       </c>
       <c r="E14" s="10">
@@ -1910,7 +1891,7 @@
       <c r="G14" s="10">
         <v>268</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="52">
         <v>268</v>
       </c>
       <c r="I14" s="5"/>
@@ -1921,16 +1902,16 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="26">
         <v>268</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="39">
         <v>268</v>
       </c>
       <c r="E15" s="10">
@@ -1942,7 +1923,7 @@
       <c r="G15" s="10">
         <v>268</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="52">
         <v>268</v>
       </c>
       <c r="I15" s="5"/>
@@ -1953,16 +1934,16 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="26">
         <v>31</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="39">
         <v>55</v>
       </c>
       <c r="E16" s="10">
@@ -1974,7 +1955,7 @@
       <c r="G16" s="10">
         <v>79</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="52">
         <v>71</v>
       </c>
       <c r="I16" s="5"/>
@@ -1985,16 +1966,16 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="26">
         <v>31</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="39">
         <v>55</v>
       </c>
       <c r="E17" s="10">
@@ -2006,7 +1987,7 @@
       <c r="G17" s="10">
         <v>79</v>
       </c>
-      <c r="H17" s="61">
+      <c r="H17" s="52">
         <v>71</v>
       </c>
       <c r="I17" s="5"/>
@@ -2017,16 +1998,16 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="26">
         <v>31</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="39">
         <v>55</v>
       </c>
       <c r="E18" s="10">
@@ -2038,7 +2019,7 @@
       <c r="G18" s="10">
         <v>79</v>
       </c>
-      <c r="H18" s="61">
+      <c r="H18" s="52">
         <v>71</v>
       </c>
       <c r="I18" s="5"/>
@@ -2049,16 +2030,16 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="26">
         <v>31</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="39">
         <v>55</v>
       </c>
       <c r="E19" s="10">
@@ -2070,7 +2051,7 @@
       <c r="G19" s="10">
         <v>79</v>
       </c>
-      <c r="H19" s="61">
+      <c r="H19" s="52">
         <v>83</v>
       </c>
       <c r="I19" s="5"/>
@@ -2081,16 +2062,16 @@
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="26">
         <v>31</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="39">
         <v>55</v>
       </c>
       <c r="E20" s="10">
@@ -2102,7 +2083,7 @@
       <c r="G20" s="10">
         <v>79</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="52">
         <v>83</v>
       </c>
       <c r="I20" s="5"/>
@@ -2113,16 +2094,16 @@
       <c r="N20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="26">
         <v>31</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="39">
         <v>63</v>
       </c>
       <c r="E21" s="10">
@@ -2134,7 +2115,7 @@
       <c r="G21" s="10">
         <v>79</v>
       </c>
-      <c r="H21" s="61">
+      <c r="H21" s="52">
         <v>83</v>
       </c>
       <c r="I21" s="5"/>
@@ -2145,16 +2126,16 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="26">
         <v>31</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="39">
         <v>67</v>
       </c>
       <c r="E22" s="10">
@@ -2166,7 +2147,7 @@
       <c r="G22" s="10">
         <v>83</v>
       </c>
-      <c r="H22" s="61">
+      <c r="H22" s="52">
         <v>83</v>
       </c>
       <c r="I22" s="5"/>
@@ -2177,16 +2158,16 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="26">
         <v>31</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="39">
         <v>67</v>
       </c>
       <c r="E23" s="10">
@@ -2198,7 +2179,7 @@
       <c r="G23" s="10">
         <v>83</v>
       </c>
-      <c r="H23" s="61">
+      <c r="H23" s="52">
         <v>83</v>
       </c>
       <c r="I23" s="5"/>
@@ -2209,16 +2190,16 @@
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="26">
         <v>31</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="39">
         <v>67</v>
       </c>
       <c r="E24" s="10">
@@ -2230,7 +2211,7 @@
       <c r="G24" s="10">
         <v>83</v>
       </c>
-      <c r="H24" s="61">
+      <c r="H24" s="52">
         <v>83</v>
       </c>
       <c r="I24" s="5"/>
@@ -2241,16 +2222,16 @@
       <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="26">
         <v>31</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="39">
         <v>67</v>
       </c>
       <c r="E25" s="10">
@@ -2262,7 +2243,7 @@
       <c r="G25" s="10">
         <v>83</v>
       </c>
-      <c r="H25" s="61">
+      <c r="H25" s="52">
         <v>83</v>
       </c>
       <c r="I25" s="5"/>
@@ -2273,33 +2254,33 @@
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="26">
         <f t="shared" ref="C26:C32" si="0">16+15</f>
         <v>31</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="39">
         <f>56+15</f>
         <v>71</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" ref="E26:E32" si="1">8+15</f>
+        <f t="shared" ref="E26:E33" si="1">8+15</f>
         <v>23</v>
       </c>
       <c r="F26" s="10">
-        <f t="shared" ref="F26:F32" si="2">88+15</f>
+        <f t="shared" ref="F26:F33" si="2">88+15</f>
         <v>103</v>
       </c>
       <c r="G26" s="10">
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H26" s="61">
+      <c r="H26" s="52">
         <f>68+15</f>
         <v>83</v>
       </c>
@@ -2311,17 +2292,17 @@
       <c r="N26" s="5"/>
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="39">
         <f>60+15</f>
         <v>75</v>
       </c>
@@ -2337,7 +2318,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H27" s="61">
+      <c r="H27" s="52">
         <f>68+15</f>
         <v>83</v>
       </c>
@@ -2349,17 +2330,17 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="39">
         <f>60+15</f>
         <v>75</v>
       </c>
@@ -2375,7 +2356,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H28" s="61">
+      <c r="H28" s="52">
         <f>52+15</f>
         <v>67</v>
       </c>
@@ -2387,17 +2368,17 @@
       <c r="N28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D29" s="48">
+      <c r="D29" s="39">
         <f>60+15</f>
         <v>75</v>
       </c>
@@ -2413,7 +2394,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H29" s="61">
+      <c r="H29" s="52">
         <f>52+15</f>
         <v>67</v>
       </c>
@@ -2425,17 +2406,17 @@
       <c r="N29" s="5"/>
     </row>
     <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="39">
         <f>60+15</f>
         <v>75</v>
       </c>
@@ -2451,7 +2432,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H30" s="61">
+      <c r="H30" s="52">
         <f>52+15</f>
         <v>67</v>
       </c>
@@ -2463,17 +2444,17 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="39">
         <f>72+15</f>
         <v>87</v>
       </c>
@@ -2489,7 +2470,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H31" s="61">
+      <c r="H31" s="52">
         <f>52+15</f>
         <v>67</v>
       </c>
@@ -2501,17 +2482,17 @@
       <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="34">
+      <c r="C32" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D32" s="48">
+      <c r="D32" s="39">
         <f>72+15</f>
         <v>87</v>
       </c>
@@ -2527,7 +2508,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H32" s="61">
+      <c r="H32" s="52">
         <f>52+15</f>
         <v>67</v>
       </c>
@@ -2538,15 +2519,35 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="61"/>
+    <row r="33" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="26">
+        <v>35</v>
+      </c>
+      <c r="D33" s="39">
+        <v>91</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="G33" s="10">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
+      <c r="H33" s="52">
+        <f>52+15</f>
+        <v>67</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2555,14 +2556,14 @@
       <c r="N33" s="5"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="29"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2607,7 +2608,7 @@
     <mergeCell ref="A10:A11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C12:C33">
+  <conditionalFormatting sqref="C12:C34">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2619,7 +2620,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D33">
+  <conditionalFormatting sqref="D12:D34">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2691,7 +2692,7 @@
     <sheetView topLeftCell="A35" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="H54" sqref="H54"/>
+      <selection pane="topRight" activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,132 +2906,132 @@
     </row>
     <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="79"/>
-      <c r="E29" s="80" t="s">
+      <c r="D29" s="85"/>
+      <c r="E29" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="80"/>
-      <c r="L29" s="80"/>
-      <c r="M29" s="80"/>
-      <c r="N29" s="77" t="s">
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="O29" s="78"/>
-      <c r="P29" s="78"/>
-      <c r="Q29" s="79"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="84"/>
+      <c r="Q29" s="85"/>
     </row>
     <row r="30" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="90" t="s">
+      <c r="A30" s="76"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="95" t="s">
+      <c r="D30" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="92" t="s">
+      <c r="E30" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83" t="s">
+      <c r="F30" s="65"/>
+      <c r="G30" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="85" t="s">
+      <c r="H30" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="83" t="s">
+      <c r="I30" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="83" t="s">
+      <c r="J30" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="K30" s="87"/>
-      <c r="L30" s="93" t="s">
+      <c r="K30" s="92"/>
+      <c r="L30" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="94"/>
-      <c r="N30" s="81" t="s">
+      <c r="M30" s="67"/>
+      <c r="N30" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="82"/>
-      <c r="P30" s="75" t="s">
+      <c r="O30" s="88"/>
+      <c r="P30" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="Q30" s="76"/>
+      <c r="Q30" s="82"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="71"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="15" t="s">
+      <c r="A31" s="77"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="84"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="84"/>
-      <c r="J31" s="16" t="s">
+      <c r="G31" s="89"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="M31" s="17" t="s">
+      <c r="M31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="N31" s="15" t="s">
+      <c r="N31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O31" s="17" t="s">
+      <c r="O31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="P31" s="15" t="s">
+      <c r="P31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="Q31" s="17" t="s">
+      <c r="Q31" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="25">
         <f>$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="D32" s="49">
+      <c r="D32" s="40">
         <f>1-(C32/$C$32)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="100">
+      <c r="E32" s="73">
         <f>$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="F32" s="97"/>
+      <c r="F32" s="74"/>
       <c r="G32" s="7">
         <f>$C$10*$C$14</f>
         <v>480</v>
@@ -3043,12 +3044,12 @@
         <f>$C$9*$C$14</f>
         <v>420</v>
       </c>
-      <c r="J32" s="105">
+      <c r="J32" s="70">
         <f>$C$11*$C$14+$C$12</f>
         <v>2936</v>
       </c>
-      <c r="K32" s="106"/>
-      <c r="L32" s="19">
+      <c r="K32" s="71"/>
+      <c r="L32" s="16">
         <f t="shared" ref="L32:L46" si="0">E32+G32+H32+I32+J32</f>
         <v>4383</v>
       </c>
@@ -3056,7 +3057,7 @@
         <f>E32+G32+H32+I32+J32</f>
         <v>4383</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="16">
         <f>7*L32</f>
         <v>30681</v>
       </c>
@@ -3064,11 +3065,11 @@
         <f>7*M32</f>
         <v>30681</v>
       </c>
-      <c r="P32" s="45">
+      <c r="P32" s="36">
         <f>1-(N32/$N$32)</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="46">
+      <c r="Q32" s="37">
         <f>1-(O32/$O$32)</f>
         <v>0</v>
       </c>
@@ -3080,25 +3081,25 @@
       <c r="W32" s="4"/>
     </row>
     <row r="33" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="26">
         <f t="shared" ref="C33:G35" si="1">$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="D33" s="50">
+      <c r="D33" s="41">
         <f t="shared" ref="D33:D45" si="2">1-(C33/$C$32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="88">
+      <c r="E33" s="60">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F33" s="89"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -3111,12 +3112,12 @@
         <f t="shared" ref="I33:I35" si="4">$C$9*$C$14</f>
         <v>420</v>
       </c>
-      <c r="J33" s="89">
+      <c r="J33" s="61">
         <f t="shared" ref="J33:J34" si="5">$C$11*$C$14+$C$12</f>
         <v>2936</v>
       </c>
-      <c r="K33" s="107"/>
-      <c r="L33" s="20">
+      <c r="K33" s="72"/>
+      <c r="L33" s="17">
         <f t="shared" si="0"/>
         <v>4383</v>
       </c>
@@ -3124,7 +3125,7 @@
         <f>E33+G33+H33+I33+J33</f>
         <v>4383</v>
       </c>
-      <c r="N33" s="20">
+      <c r="N33" s="17">
         <f t="shared" ref="N33:N46" si="6">7*L33</f>
         <v>30681</v>
       </c>
@@ -3132,11 +3133,11 @@
         <f t="shared" ref="O33:O51" si="7">7*M33</f>
         <v>30681</v>
       </c>
-      <c r="P33" s="45">
+      <c r="P33" s="36">
         <f t="shared" ref="P33:P51" si="8">1-(N33/$N$32)</f>
         <v>0</v>
       </c>
-      <c r="Q33" s="46">
+      <c r="Q33" s="37">
         <f t="shared" ref="Q33:Q51" si="9">1-(O33/$O$32)</f>
         <v>0</v>
       </c>
@@ -3148,25 +3149,25 @@
       <c r="W33" s="4"/>
     </row>
     <row r="34" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="26">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D34" s="50">
+      <c r="D34" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E34" s="88">
+      <c r="E34" s="60">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F34" s="89"/>
+      <c r="F34" s="61"/>
       <c r="G34" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -3179,12 +3180,12 @@
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J34" s="89">
+      <c r="J34" s="61">
         <f t="shared" si="5"/>
         <v>2936</v>
       </c>
-      <c r="K34" s="107"/>
-      <c r="L34" s="20">
+      <c r="K34" s="72"/>
+      <c r="L34" s="17">
         <f t="shared" si="0"/>
         <v>4383</v>
       </c>
@@ -3192,7 +3193,7 @@
         <f>E34+G34+H34+I34+J34</f>
         <v>4383</v>
       </c>
-      <c r="N34" s="20">
+      <c r="N34" s="17">
         <f t="shared" si="6"/>
         <v>30681</v>
       </c>
@@ -3200,11 +3201,11 @@
         <f t="shared" si="7"/>
         <v>30681</v>
       </c>
-      <c r="P34" s="45">
+      <c r="P34" s="36">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q34" s="46">
+      <c r="Q34" s="37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3216,25 +3217,25 @@
       <c r="W34" s="4"/>
     </row>
     <row r="35" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="26">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D35" s="50">
+      <c r="D35" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E35" s="88">
+      <c r="E35" s="60">
         <f>$C$10*$C$16</f>
         <v>160</v>
       </c>
-      <c r="F35" s="89"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="10">
         <f>$C$10*$C$16</f>
         <v>160</v>
@@ -3251,11 +3252,11 @@
         <f>$C$11*$C$16+$C$12</f>
         <v>1016</v>
       </c>
-      <c r="K35" s="18">
+      <c r="K35" s="15">
         <f>$C$11*$C$16+$C$12</f>
         <v>1016</v>
       </c>
-      <c r="L35" s="20">
+      <c r="L35" s="17">
         <f t="shared" si="0"/>
         <v>1783</v>
       </c>
@@ -3263,7 +3264,7 @@
         <f>E35+G35+H35+I35+K35</f>
         <v>1783</v>
       </c>
-      <c r="N35" s="20">
+      <c r="N35" s="17">
         <f t="shared" si="6"/>
         <v>12481</v>
       </c>
@@ -3271,11 +3272,11 @@
         <f t="shared" si="7"/>
         <v>12481</v>
       </c>
-      <c r="P35" s="45">
+      <c r="P35" s="36">
         <f t="shared" si="8"/>
         <v>0.59320100387862196</v>
       </c>
-      <c r="Q35" s="46">
+      <c r="Q35" s="37">
         <f t="shared" si="9"/>
         <v>0.59320100387862196</v>
       </c>
@@ -3287,25 +3288,25 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="34">
+      <c r="C36" s="26">
         <f>16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D36" s="50">
+      <c r="D36" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
-      <c r="E36" s="88">
+      <c r="E36" s="60">
         <f t="shared" ref="E36" si="10">$C$10*$C$16</f>
         <v>160</v>
       </c>
-      <c r="F36" s="89"/>
+      <c r="F36" s="61"/>
       <c r="G36" s="10">
         <f>$C$10*$C$16</f>
         <v>160</v>
@@ -3322,11 +3323,11 @@
         <f>$C$12</f>
         <v>56</v>
       </c>
-      <c r="K36" s="18">
+      <c r="K36" s="15">
         <f>$C$12</f>
         <v>56</v>
       </c>
-      <c r="L36" s="20">
+      <c r="L36" s="17">
         <f t="shared" si="0"/>
         <v>417</v>
       </c>
@@ -3334,7 +3335,7 @@
         <f>E36+G36+H36+I36+K36</f>
         <v>417</v>
       </c>
-      <c r="N36" s="20">
+      <c r="N36" s="17">
         <f t="shared" si="6"/>
         <v>2919</v>
       </c>
@@ -3342,11 +3343,11 @@
         <f t="shared" si="7"/>
         <v>2919</v>
       </c>
-      <c r="P36" s="45">
+      <c r="P36" s="36">
         <f t="shared" si="8"/>
         <v>0.90485968514715953</v>
       </c>
-      <c r="Q36" s="46">
+      <c r="Q36" s="37">
         <f t="shared" si="9"/>
         <v>0.90485968514715953</v>
       </c>
@@ -3358,17 +3359,17 @@
       <c r="W36" s="4"/>
     </row>
     <row r="37" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="34">
-        <f t="shared" ref="C37:C52" si="11">16*$C$10</f>
+      <c r="C37" s="26">
+        <f t="shared" ref="C37:C53" si="11">16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3377,14 +3378,14 @@
         <v>160</v>
       </c>
       <c r="F37" s="10">
-        <f t="shared" ref="F37:F52" si="12">$C$10*$C$17</f>
+        <f t="shared" ref="F37:F53" si="12">$C$10*$C$17</f>
         <v>480</v>
       </c>
       <c r="G37" s="10">
         <f>$C$10*$C$15</f>
         <v>480</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H37" s="15">
         <f>7 + 1*$C$14</f>
         <v>67</v>
       </c>
@@ -3393,14 +3394,14 @@
         <v>14</v>
       </c>
       <c r="J37" s="10">
-        <f t="shared" ref="J37:K52" si="14">$C$12</f>
+        <f t="shared" ref="J37:K51" si="14">$C$12</f>
         <v>56</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L37" s="20">
+      <c r="L37" s="17">
         <f t="shared" si="0"/>
         <v>777</v>
       </c>
@@ -3408,7 +3409,7 @@
         <f t="shared" ref="M37:M51" si="15">F37+G37+H37+I37+K37</f>
         <v>1097</v>
       </c>
-      <c r="N37" s="20">
+      <c r="N37" s="17">
         <f t="shared" si="6"/>
         <v>5439</v>
       </c>
@@ -3416,11 +3417,11 @@
         <f t="shared" si="7"/>
         <v>7679</v>
       </c>
-      <c r="P37" s="45">
+      <c r="P37" s="36">
         <f t="shared" si="8"/>
         <v>0.82272416153319639</v>
       </c>
-      <c r="Q37" s="46">
+      <c r="Q37" s="37">
         <f t="shared" si="9"/>
         <v>0.74971480720967376</v>
       </c>
@@ -3432,22 +3433,22 @@
       <c r="W37" s="4"/>
     </row>
     <row r="38" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D38" s="50">
+      <c r="D38" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
       <c r="E38" s="9">
-        <f t="shared" ref="E38:E52" si="16">$C$10*$C$18</f>
+        <f t="shared" ref="E38:E53" si="16">$C$10*$C$18</f>
         <v>160</v>
       </c>
       <c r="F38" s="10">
@@ -3455,11 +3456,11 @@
         <v>480</v>
       </c>
       <c r="G38" s="10">
-        <f t="shared" ref="G38:G52" si="17">$C$10*$C$15</f>
+        <f t="shared" ref="G38:G53" si="17">$C$10*$C$15</f>
         <v>480</v>
       </c>
-      <c r="H38" s="18">
-        <f t="shared" ref="H38:H52" si="18">7 + 1*$C$14</f>
+      <c r="H38" s="15">
+        <f t="shared" ref="H38:H53" si="18">7 + 1*$C$14</f>
         <v>67</v>
       </c>
       <c r="I38" s="10">
@@ -3470,11 +3471,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L38" s="20">
+      <c r="L38" s="17">
         <f t="shared" si="0"/>
         <v>777</v>
       </c>
@@ -3482,7 +3483,7 @@
         <f t="shared" si="15"/>
         <v>1097</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N38" s="17">
         <f t="shared" si="6"/>
         <v>5439</v>
       </c>
@@ -3490,11 +3491,11 @@
         <f t="shared" si="7"/>
         <v>7679</v>
       </c>
-      <c r="P38" s="45">
+      <c r="P38" s="36">
         <f t="shared" si="8"/>
         <v>0.82272416153319639</v>
       </c>
-      <c r="Q38" s="46">
+      <c r="Q38" s="37">
         <f t="shared" si="9"/>
         <v>0.74971480720967376</v>
       </c>
@@ -3506,17 +3507,17 @@
       <c r="W38" s="4"/>
     </row>
     <row r="39" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C39" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D39" s="50">
+      <c r="D39" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3532,7 +3533,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3544,11 +3545,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L39" s="20">
+      <c r="L39" s="17">
         <f t="shared" si="0"/>
         <v>777</v>
       </c>
@@ -3556,7 +3557,7 @@
         <f t="shared" si="15"/>
         <v>1097</v>
       </c>
-      <c r="N39" s="20">
+      <c r="N39" s="17">
         <f t="shared" si="6"/>
         <v>5439</v>
       </c>
@@ -3564,11 +3565,11 @@
         <f t="shared" si="7"/>
         <v>7679</v>
       </c>
-      <c r="P39" s="45">
+      <c r="P39" s="36">
         <f t="shared" si="8"/>
         <v>0.82272416153319639</v>
       </c>
-      <c r="Q39" s="46">
+      <c r="Q39" s="37">
         <f t="shared" si="9"/>
         <v>0.74971480720967376</v>
       </c>
@@ -3580,17 +3581,17 @@
       <c r="W39" s="4"/>
     </row>
     <row r="40" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="34">
+      <c r="C40" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D40" s="50">
+      <c r="D40" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3606,7 +3607,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H40" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3618,11 +3619,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K40" s="18">
+      <c r="K40" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L40" s="20">
+      <c r="L40" s="17">
         <f t="shared" si="0"/>
         <v>777</v>
       </c>
@@ -3630,7 +3631,7 @@
         <f t="shared" si="15"/>
         <v>1097</v>
       </c>
-      <c r="N40" s="20">
+      <c r="N40" s="17">
         <f t="shared" si="6"/>
         <v>5439</v>
       </c>
@@ -3638,11 +3639,11 @@
         <f t="shared" si="7"/>
         <v>7679</v>
       </c>
-      <c r="P40" s="45">
+      <c r="P40" s="36">
         <f t="shared" si="8"/>
         <v>0.82272416153319639</v>
       </c>
-      <c r="Q40" s="46">
+      <c r="Q40" s="37">
         <f t="shared" si="9"/>
         <v>0.74971480720967376</v>
       </c>
@@ -3654,17 +3655,17 @@
       <c r="W40" s="4"/>
     </row>
     <row r="41" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="34">
+      <c r="C41" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D41" s="50">
+      <c r="D41" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3680,7 +3681,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H41" s="18">
+      <c r="H41" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3692,11 +3693,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K41" s="18">
+      <c r="K41" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L41" s="20">
+      <c r="L41" s="17">
         <f t="shared" si="0"/>
         <v>777</v>
       </c>
@@ -3704,7 +3705,7 @@
         <f t="shared" si="15"/>
         <v>1097</v>
       </c>
-      <c r="N41" s="20">
+      <c r="N41" s="17">
         <f t="shared" si="6"/>
         <v>5439</v>
       </c>
@@ -3712,11 +3713,11 @@
         <f t="shared" si="7"/>
         <v>7679</v>
       </c>
-      <c r="P41" s="45">
+      <c r="P41" s="36">
         <f t="shared" si="8"/>
         <v>0.82272416153319639</v>
       </c>
-      <c r="Q41" s="46">
+      <c r="Q41" s="37">
         <f t="shared" si="9"/>
         <v>0.74971480720967376</v>
       </c>
@@ -3728,17 +3729,17 @@
       <c r="W41" s="4"/>
     </row>
     <row r="42" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="34">
+      <c r="C42" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D42" s="50">
+      <c r="D42" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3754,7 +3755,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H42" s="18">
+      <c r="H42" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3766,11 +3767,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K42" s="18">
+      <c r="K42" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L42" s="20">
+      <c r="L42" s="17">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
@@ -3778,7 +3779,7 @@
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N42" s="20">
+      <c r="N42" s="17">
         <f t="shared" si="6"/>
         <v>5537</v>
       </c>
@@ -3786,11 +3787,11 @@
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P42" s="45">
+      <c r="P42" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q42" s="46">
+      <c r="Q42" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -3802,17 +3803,17 @@
       <c r="W42" s="4"/>
     </row>
     <row r="43" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="34">
+      <c r="C43" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D43" s="50">
+      <c r="D43" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3828,23 +3829,23 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
       <c r="I43" s="10">
-        <f t="shared" ref="I43:I52" si="19">$C$9*2 + $C$9*2</f>
+        <f t="shared" ref="I43:I53" si="19">$C$9*2 + $C$9*2</f>
         <v>28</v>
       </c>
       <c r="J43" s="10">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K43" s="18">
+      <c r="K43" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L43" s="20">
+      <c r="L43" s="17">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
@@ -3852,7 +3853,7 @@
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N43" s="20">
+      <c r="N43" s="17">
         <f t="shared" si="6"/>
         <v>5537</v>
       </c>
@@ -3860,11 +3861,11 @@
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P43" s="45">
+      <c r="P43" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q43" s="46">
+      <c r="Q43" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -3876,17 +3877,17 @@
       <c r="W43" s="4"/>
     </row>
     <row r="44" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="34">
+      <c r="C44" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3902,7 +3903,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3914,11 +3915,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K44" s="18">
+      <c r="K44" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L44" s="20">
+      <c r="L44" s="17">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
@@ -3926,7 +3927,7 @@
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N44" s="20">
+      <c r="N44" s="17">
         <f t="shared" si="6"/>
         <v>5537</v>
       </c>
@@ -3934,11 +3935,11 @@
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P44" s="45">
+      <c r="P44" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q44" s="46">
+      <c r="Q44" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -3950,17 +3951,17 @@
       <c r="W44" s="4"/>
     </row>
     <row r="45" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="34">
+      <c r="C45" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D45" s="50">
+      <c r="D45" s="41">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3976,7 +3977,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -3988,11 +3989,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L45" s="20">
+      <c r="L45" s="17">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
@@ -4000,7 +4001,7 @@
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N45" s="20">
+      <c r="N45" s="17">
         <f t="shared" si="6"/>
         <v>5537</v>
       </c>
@@ -4008,11 +4009,11 @@
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P45" s="45">
+      <c r="P45" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q45" s="46">
+      <c r="Q45" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4024,17 +4025,17 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="34">
+      <c r="C46" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D46" s="50">
+      <c r="D46" s="41">
         <f t="shared" ref="D46:D52" si="20">1-(C46/$C$32)</f>
         <v>0.73333333333333339</v>
       </c>
@@ -4050,7 +4051,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4062,11 +4063,11 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K46" s="18">
+      <c r="K46" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L46" s="20">
+      <c r="L46" s="17">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
@@ -4074,7 +4075,7 @@
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N46" s="20">
+      <c r="N46" s="17">
         <f t="shared" si="6"/>
         <v>5537</v>
       </c>
@@ -4082,11 +4083,11 @@
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P46" s="45">
+      <c r="P46" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q46" s="46">
+      <c r="Q46" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4098,17 +4099,17 @@
       <c r="W46" s="4"/>
     </row>
     <row r="47" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="34">
+      <c r="C47" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4124,7 +4125,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4136,31 +4137,31 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K47" s="18">
+      <c r="K47" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L47" s="20">
-        <f>E47+G47+H47+I47+J47</f>
+      <c r="L47" s="17">
+        <f t="shared" ref="L47:L52" si="21">E47+G47+H47+I47+J47</f>
         <v>791</v>
       </c>
       <c r="M47" s="11">
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N47" s="20">
-        <f>7*L47</f>
+      <c r="N47" s="17">
+        <f t="shared" ref="N47:N52" si="22">7*L47</f>
         <v>5537</v>
       </c>
       <c r="O47" s="11">
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P47" s="45">
+      <c r="P47" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q47" s="46">
+      <c r="Q47" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4172,17 +4173,17 @@
       <c r="W47" s="4"/>
     </row>
     <row r="48" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D48" s="50">
+      <c r="D48" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4198,7 +4199,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4210,31 +4211,31 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K48" s="18">
+      <c r="K48" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L48" s="20">
-        <f>E48+G48+H48+I48+J48</f>
+      <c r="L48" s="17">
+        <f t="shared" si="21"/>
         <v>791</v>
       </c>
       <c r="M48" s="11">
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N48" s="20">
-        <f>7*L48</f>
+      <c r="N48" s="17">
+        <f t="shared" si="22"/>
         <v>5537</v>
       </c>
       <c r="O48" s="11">
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P48" s="45">
+      <c r="P48" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q48" s="46">
+      <c r="Q48" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4246,17 +4247,17 @@
       <c r="W48" s="4"/>
     </row>
     <row r="49" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="34">
+      <c r="C49" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D49" s="50">
+      <c r="D49" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4272,7 +4273,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4284,31 +4285,31 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L49" s="20">
-        <f>E49+G49+H49+I49+J49</f>
+      <c r="L49" s="17">
+        <f t="shared" si="21"/>
         <v>791</v>
       </c>
       <c r="M49" s="11">
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N49" s="20">
-        <f>7*L49</f>
+      <c r="N49" s="17">
+        <f t="shared" si="22"/>
         <v>5537</v>
       </c>
       <c r="O49" s="11">
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P49" s="45">
+      <c r="P49" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q49" s="46">
+      <c r="Q49" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4320,17 +4321,17 @@
       <c r="W49" s="4"/>
     </row>
     <row r="50" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="34">
+      <c r="C50" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D50" s="50">
+      <c r="D50" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4346,7 +4347,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H50" s="18">
+      <c r="H50" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4358,31 +4359,31 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K50" s="18">
+      <c r="K50" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L50" s="20">
-        <f>E50+G50+H50+I50+J50</f>
+      <c r="L50" s="17">
+        <f t="shared" si="21"/>
         <v>791</v>
       </c>
       <c r="M50" s="11">
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N50" s="20">
-        <f>7*L50</f>
+      <c r="N50" s="17">
+        <f t="shared" si="22"/>
         <v>5537</v>
       </c>
       <c r="O50" s="11">
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P50" s="45">
+      <c r="P50" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q50" s="46">
+      <c r="Q50" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4394,17 +4395,17 @@
       <c r="W50" s="4"/>
     </row>
     <row r="51" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C51" s="34">
+      <c r="C51" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D51" s="50">
+      <c r="D51" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4420,7 +4421,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H51" s="18">
+      <c r="H51" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4432,31 +4433,31 @@
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="K51" s="18">
+      <c r="K51" s="15">
         <f t="shared" si="14"/>
         <v>56</v>
       </c>
-      <c r="L51" s="20">
-        <f>E51+G51+H51+I51+J51</f>
+      <c r="L51" s="17">
+        <f t="shared" si="21"/>
         <v>791</v>
       </c>
       <c r="M51" s="11">
         <f t="shared" si="15"/>
         <v>1111</v>
       </c>
-      <c r="N51" s="20">
-        <f>7*L51</f>
+      <c r="N51" s="17">
+        <f t="shared" si="22"/>
         <v>5537</v>
       </c>
       <c r="O51" s="11">
         <f t="shared" si="7"/>
         <v>7777</v>
       </c>
-      <c r="P51" s="45">
+      <c r="P51" s="36">
         <f t="shared" si="8"/>
         <v>0.81953000228154238</v>
       </c>
-      <c r="Q51" s="46">
+      <c r="Q51" s="37">
         <f t="shared" si="9"/>
         <v>0.74652064795801965</v>
       </c>
@@ -4468,17 +4469,17 @@
       <c r="W51" s="4"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52" s="26">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D52" s="50">
+      <c r="D52" s="41">
         <f t="shared" si="20"/>
         <v>0.73333333333333339</v>
       </c>
@@ -4494,7 +4495,7 @@
         <f t="shared" si="17"/>
         <v>480</v>
       </c>
-      <c r="H52" s="18">
+      <c r="H52" s="15">
         <f t="shared" si="18"/>
         <v>67</v>
       </c>
@@ -4506,32 +4507,32 @@
         <f>$C$21</f>
         <v>160</v>
       </c>
-      <c r="K52" s="18">
+      <c r="K52" s="15">
         <f>$C$21</f>
         <v>160</v>
       </c>
-      <c r="L52" s="20">
-        <f>E52+G52+H52+I52+J52</f>
+      <c r="L52" s="17">
+        <f t="shared" si="21"/>
         <v>895</v>
       </c>
       <c r="M52" s="11">
-        <f t="shared" ref="M52" si="21">F52+G52+H52+I52+K52</f>
+        <f t="shared" ref="M52" si="23">F52+G52+H52+I52+K52</f>
         <v>1215</v>
       </c>
-      <c r="N52" s="20">
-        <f>7*L52</f>
+      <c r="N52" s="17">
+        <f t="shared" si="22"/>
         <v>6265</v>
       </c>
       <c r="O52" s="11">
-        <f t="shared" ref="O52" si="22">7*M52</f>
+        <f t="shared" ref="O52" si="24">7*M52</f>
         <v>8505</v>
       </c>
-      <c r="P52" s="45">
-        <f t="shared" ref="P52" si="23">1-(N52/$N$32)</f>
+      <c r="P52" s="36">
+        <f t="shared" ref="P52" si="25">1-(N52/$N$32)</f>
         <v>0.79580196212639742</v>
       </c>
-      <c r="Q52" s="46">
-        <f t="shared" ref="Q52" si="24">1-(O52/$O$32)</f>
+      <c r="Q52" s="37">
+        <f t="shared" ref="Q52" si="26">1-(O52/$O$32)</f>
         <v>0.7227926078028748</v>
       </c>
       <c r="R52" s="4"/>
@@ -4542,23 +4543,72 @@
       <c r="W52" s="4"/>
     </row>
     <row r="53" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="21"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="45"/>
-      <c r="Q53" s="46"/>
+      <c r="A53" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="26">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+      <c r="D53" s="41">
+        <f t="shared" ref="D53" si="27">1-(C53/$C$32)</f>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="E53" s="9">
+        <f t="shared" si="16"/>
+        <v>160</v>
+      </c>
+      <c r="F53" s="10">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="G53" s="10">
+        <f t="shared" si="17"/>
+        <v>480</v>
+      </c>
+      <c r="H53" s="15">
+        <f t="shared" si="18"/>
+        <v>67</v>
+      </c>
+      <c r="I53" s="10">
+        <f t="shared" si="19"/>
+        <v>28</v>
+      </c>
+      <c r="J53" s="10">
+        <f>$C$21</f>
+        <v>160</v>
+      </c>
+      <c r="K53" s="15">
+        <f>$C$21</f>
+        <v>160</v>
+      </c>
+      <c r="L53" s="17">
+        <f t="shared" ref="L53" si="28">E53+G53+H53+I53+J53</f>
+        <v>895</v>
+      </c>
+      <c r="M53" s="11">
+        <f t="shared" ref="M53" si="29">F53+G53+H53+I53+K53</f>
+        <v>1215</v>
+      </c>
+      <c r="N53" s="17">
+        <f t="shared" ref="N53" si="30">7*L53</f>
+        <v>6265</v>
+      </c>
+      <c r="O53" s="11">
+        <f t="shared" ref="O53" si="31">7*M53</f>
+        <v>8505</v>
+      </c>
+      <c r="P53" s="36">
+        <f t="shared" ref="P53" si="32">1-(N53/$N$32)</f>
+        <v>0.79580196212639742</v>
+      </c>
+      <c r="Q53" s="37">
+        <f t="shared" ref="Q53" si="33">1-(O53/$O$32)</f>
+        <v>0.7227926078028748</v>
+      </c>
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
       <c r="T53" s="4"/>
@@ -4569,7 +4619,7 @@
     <row r="54" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="C54" s="4"/>
-      <c r="D54" s="51"/>
+      <c r="D54" s="42"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -4581,8 +4631,8 @@
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
-      <c r="P54" s="47"/>
-      <c r="Q54" s="47"/>
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38"/>
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
       <c r="T54" s="4"/>
@@ -4649,6 +4699,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="E29:M29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C30:C31"/>
@@ -4661,18 +4722,8 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="E29:M29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="C29:D29"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C32:D53">
     <cfRule type="colorScale" priority="17">
       <colorScale>
@@ -4769,7 +4820,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N32:O52">
+  <conditionalFormatting sqref="N32:O53">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4781,7 +4832,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P32:Q52">
+  <conditionalFormatting sqref="P32:Q53">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4802,9 +4853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A631036-56BD-4CE5-917C-895C0C771D72}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R36" sqref="R36"/>
+      <selection pane="topRight" activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,132 +4923,132 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80" t="s">
+      <c r="D15" s="85"/>
+      <c r="E15" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="77" t="s">
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="79"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="85"/>
     </row>
     <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="90" t="s">
+      <c r="A16" s="76"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="92" t="s">
+      <c r="E16" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83" t="s">
+      <c r="F16" s="65"/>
+      <c r="G16" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="85" t="s">
+      <c r="H16" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="83" t="s">
+      <c r="I16" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="83" t="s">
+      <c r="J16" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="87"/>
-      <c r="L16" s="93" t="s">
+      <c r="K16" s="92"/>
+      <c r="L16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="94"/>
-      <c r="N16" s="81" t="s">
+      <c r="M16" s="67"/>
+      <c r="N16" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="82"/>
-      <c r="P16" s="75" t="s">
+      <c r="O16" s="88"/>
+      <c r="P16" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="Q16" s="76"/>
+      <c r="Q16" s="82"/>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="15" t="s">
+      <c r="A17" s="77"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="84"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="16" t="s">
+      <c r="G17" s="89"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="O17" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="P17" s="15" t="s">
+      <c r="P17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" s="17" t="s">
+      <c r="Q17" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="25">
         <f>'Packet Rates'!C32*'Packet Sizes'!C12</f>
         <v>128640</v>
       </c>
-      <c r="D18" s="52">
+      <c r="D18" s="43">
         <f>1-(C18/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="101">
+      <c r="E18" s="93">
         <f>'Packet Rates'!E32*'Packet Sizes'!D12</f>
         <v>128640</v>
       </c>
-      <c r="F18" s="102"/>
+      <c r="F18" s="94"/>
       <c r="G18" s="7">
         <f>'Packet Rates'!G32*'Packet Sizes'!E12</f>
         <v>128640</v>
@@ -5010,12 +5061,12 @@
         <f>'Packet Rates'!I32*'Packet Sizes'!G12</f>
         <v>112560</v>
       </c>
-      <c r="J18" s="97">
+      <c r="J18" s="74">
         <f>'Packet Rates'!J32*'Packet Sizes'!H12</f>
         <v>786848</v>
       </c>
-      <c r="K18" s="98"/>
-      <c r="L18" s="19">
+      <c r="K18" s="95"/>
+      <c r="L18" s="16">
         <f>E18+G18+H18+I18+J18</f>
         <v>1174644</v>
       </c>
@@ -5023,7 +5074,7 @@
         <f>E18+G18+H18+I18+J18</f>
         <v>1174644</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="16">
         <f>L18*7</f>
         <v>8222508</v>
       </c>
@@ -5031,35 +5082,35 @@
         <f>M18*7</f>
         <v>8222508</v>
       </c>
-      <c r="P18" s="45">
+      <c r="P18" s="36">
         <f>1-(N18/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="46">
+      <c r="Q18" s="37">
         <f>1-(O18/$O$18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="26">
         <f>'Packet Rates'!C33*'Packet Sizes'!C13</f>
         <v>128640</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="44">
         <f t="shared" ref="D19:D33" si="0">1-(C19/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="103">
+      <c r="E19" s="96">
         <f>'Packet Rates'!E33*'Packet Sizes'!D13</f>
         <v>128640</v>
       </c>
-      <c r="F19" s="104"/>
+      <c r="F19" s="97"/>
       <c r="G19" s="10">
         <f>'Packet Rates'!G33*'Packet Sizes'!E13</f>
         <v>128640</v>
@@ -5072,12 +5123,12 @@
         <f>'Packet Rates'!I33*'Packet Sizes'!G13</f>
         <v>112560</v>
       </c>
-      <c r="J19" s="89">
+      <c r="J19" s="61">
         <f>'Packet Rates'!J33*'Packet Sizes'!H13</f>
         <v>786848</v>
       </c>
-      <c r="K19" s="99"/>
-      <c r="L19" s="20">
+      <c r="K19" s="98"/>
+      <c r="L19" s="17">
         <f t="shared" ref="L19:L33" si="1">E19+G19+H19+I19+J19</f>
         <v>1174644</v>
       </c>
@@ -5085,7 +5136,7 @@
         <f t="shared" ref="M19:M20" si="2">E19+G19+H19+I19+J19</f>
         <v>1174644</v>
       </c>
-      <c r="N19" s="20">
+      <c r="N19" s="17">
         <f t="shared" ref="N19:N33" si="3">L19*7</f>
         <v>8222508</v>
       </c>
@@ -5093,35 +5144,35 @@
         <f t="shared" ref="O19:O33" si="4">M19*7</f>
         <v>8222508</v>
       </c>
-      <c r="P19" s="45">
+      <c r="P19" s="36">
         <f t="shared" ref="P19:P33" si="5">1-(N19/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="46">
+      <c r="Q19" s="37">
         <f t="shared" ref="Q19:Q33" si="6">1-(O19/$O$18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="26">
         <f>'Packet Rates'!C34*'Packet Sizes'!C14</f>
         <v>128640</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="103">
+      <c r="E20" s="96">
         <f>'Packet Rates'!E34*'Packet Sizes'!D14</f>
         <v>128640</v>
       </c>
-      <c r="F20" s="104"/>
+      <c r="F20" s="97"/>
       <c r="G20" s="10">
         <f>'Packet Rates'!G34*'Packet Sizes'!E14</f>
         <v>128640</v>
@@ -5134,12 +5185,12 @@
         <f>'Packet Rates'!I34*'Packet Sizes'!G14</f>
         <v>112560</v>
       </c>
-      <c r="J20" s="89">
+      <c r="J20" s="61">
         <f>'Packet Rates'!J34*'Packet Sizes'!H14</f>
         <v>786848</v>
       </c>
-      <c r="K20" s="99"/>
-      <c r="L20" s="20">
+      <c r="K20" s="98"/>
+      <c r="L20" s="17">
         <f t="shared" si="1"/>
         <v>1174644</v>
       </c>
@@ -5147,7 +5198,7 @@
         <f t="shared" si="2"/>
         <v>1174644</v>
       </c>
-      <c r="N20" s="20">
+      <c r="N20" s="17">
         <f t="shared" si="3"/>
         <v>8222508</v>
       </c>
@@ -5155,35 +5206,35 @@
         <f t="shared" si="4"/>
         <v>8222508</v>
       </c>
-      <c r="P20" s="45">
+      <c r="P20" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="46">
+      <c r="Q20" s="37">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="26">
         <f>'Packet Rates'!C35*'Packet Sizes'!C15</f>
         <v>128640</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="88">
+      <c r="E21" s="60">
         <f>'Packet Rates'!E35*'Packet Sizes'!D15</f>
         <v>42880</v>
       </c>
-      <c r="F21" s="89"/>
+      <c r="F21" s="61"/>
       <c r="G21" s="10">
         <f>'Packet Rates'!G35*'Packet Sizes'!E15</f>
         <v>42880</v>
@@ -5200,11 +5251,11 @@
         <f>'Packet Rates'!J35*'Packet Sizes'!H15</f>
         <v>272288</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="15">
         <f>'Packet Rates'!K35*'Packet Sizes'!H15</f>
         <v>272288</v>
       </c>
-      <c r="L21" s="20">
+      <c r="L21" s="17">
         <f t="shared" si="1"/>
         <v>477844</v>
       </c>
@@ -5212,7 +5263,7 @@
         <f>E21+G21+H21+I21+K21</f>
         <v>477844</v>
       </c>
-      <c r="N21" s="20">
+      <c r="N21" s="17">
         <f t="shared" si="3"/>
         <v>3344908</v>
       </c>
@@ -5220,35 +5271,35 @@
         <f t="shared" si="4"/>
         <v>3344908</v>
       </c>
-      <c r="P21" s="45">
+      <c r="P21" s="36">
         <f t="shared" si="5"/>
         <v>0.59320100387862196</v>
       </c>
-      <c r="Q21" s="46">
+      <c r="Q21" s="37">
         <f t="shared" si="6"/>
         <v>0.59320100387862196</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="26">
         <f>'Packet Rates'!C36*'Packet Sizes'!C16</f>
         <v>3968</v>
       </c>
-      <c r="D22" s="53">
+      <c r="D22" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
-      <c r="E22" s="88">
+      <c r="E22" s="60">
         <f>'Packet Rates'!E36*'Packet Sizes'!D16</f>
         <v>8800</v>
       </c>
-      <c r="F22" s="89"/>
+      <c r="F22" s="61"/>
       <c r="G22" s="10">
         <f>'Packet Rates'!G36*'Packet Sizes'!E16</f>
         <v>3680</v>
@@ -5265,11 +5316,11 @@
         <f>'Packet Rates'!J36*'Packet Sizes'!H16</f>
         <v>3976</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="15">
         <f>'Packet Rates'!K36*'Packet Sizes'!H16</f>
         <v>3976</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="17">
         <f t="shared" si="1"/>
         <v>20019</v>
       </c>
@@ -5277,7 +5328,7 @@
         <f>E22+G22+H22+I22+K22</f>
         <v>20019</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="17">
         <f t="shared" si="3"/>
         <v>140133</v>
       </c>
@@ -5285,27 +5336,27 @@
         <f t="shared" si="4"/>
         <v>140133</v>
       </c>
-      <c r="P22" s="45">
+      <c r="P22" s="36">
         <f t="shared" si="5"/>
         <v>0.98295738964315993</v>
       </c>
-      <c r="Q22" s="46">
+      <c r="Q22" s="37">
         <f t="shared" si="6"/>
         <v>0.98295738964315993</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="26">
         <f>'Packet Rates'!C37*'Packet Sizes'!C17</f>
         <v>3968</v>
       </c>
-      <c r="D23" s="53">
+      <c r="D23" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5333,11 +5384,11 @@
         <f>'Packet Rates'!J37*'Packet Sizes'!H17</f>
         <v>3976</v>
       </c>
-      <c r="K23" s="18">
+      <c r="K23" s="15">
         <f>'Packet Rates'!K37*'Packet Sizes'!H17</f>
         <v>3976</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L23" s="17">
         <f t="shared" si="1"/>
         <v>31019</v>
       </c>
@@ -5345,7 +5396,7 @@
         <f>F23+G23+H23+I23+K23</f>
         <v>48619</v>
       </c>
-      <c r="N23" s="20">
+      <c r="N23" s="17">
         <f t="shared" si="3"/>
         <v>217133</v>
       </c>
@@ -5353,27 +5404,27 @@
         <f t="shared" si="4"/>
         <v>340333</v>
       </c>
-      <c r="P23" s="45">
+      <c r="P23" s="36">
         <f t="shared" si="5"/>
         <v>0.97359285025931264</v>
       </c>
-      <c r="Q23" s="46">
+      <c r="Q23" s="37">
         <f t="shared" si="6"/>
         <v>0.95860958724515688</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="26">
         <f>'Packet Rates'!C38*'Packet Sizes'!C18</f>
         <v>3968</v>
       </c>
-      <c r="D24" s="53">
+      <c r="D24" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5401,11 +5452,11 @@
         <f>'Packet Rates'!J38*'Packet Sizes'!H18</f>
         <v>3976</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="15">
         <f>'Packet Rates'!K38*'Packet Sizes'!H18</f>
         <v>3976</v>
       </c>
-      <c r="L24" s="20">
+      <c r="L24" s="17">
         <f t="shared" si="1"/>
         <v>31019</v>
       </c>
@@ -5413,7 +5464,7 @@
         <f t="shared" ref="M24:M33" si="7">F24+G24+H24+I24+K24</f>
         <v>48619</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="17">
         <f t="shared" si="3"/>
         <v>217133</v>
       </c>
@@ -5421,27 +5472,27 @@
         <f t="shared" si="4"/>
         <v>340333</v>
       </c>
-      <c r="P24" s="45">
+      <c r="P24" s="36">
         <f t="shared" si="5"/>
         <v>0.97359285025931264</v>
       </c>
-      <c r="Q24" s="46">
+      <c r="Q24" s="37">
         <f t="shared" si="6"/>
         <v>0.95860958724515688</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="26">
         <f>'Packet Rates'!C39*'Packet Sizes'!C19</f>
         <v>3968</v>
       </c>
-      <c r="D25" s="53">
+      <c r="D25" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5469,11 +5520,11 @@
         <f>'Packet Rates'!J39*'Packet Sizes'!H19</f>
         <v>4648</v>
       </c>
-      <c r="K25" s="18">
+      <c r="K25" s="15">
         <f>'Packet Rates'!K39*'Packet Sizes'!H19</f>
         <v>4648</v>
       </c>
-      <c r="L25" s="20">
+      <c r="L25" s="17">
         <f t="shared" si="1"/>
         <v>31691</v>
       </c>
@@ -5481,7 +5532,7 @@
         <f t="shared" si="7"/>
         <v>49291</v>
       </c>
-      <c r="N25" s="20">
+      <c r="N25" s="17">
         <f t="shared" si="3"/>
         <v>221837</v>
       </c>
@@ -5489,27 +5540,27 @@
         <f t="shared" si="4"/>
         <v>345037</v>
       </c>
-      <c r="P25" s="45">
+      <c r="P25" s="36">
         <f t="shared" si="5"/>
         <v>0.97302076203513577</v>
       </c>
-      <c r="Q25" s="46">
+      <c r="Q25" s="37">
         <f t="shared" si="6"/>
         <v>0.95803749902098001</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="26">
         <f>'Packet Rates'!C40*'Packet Sizes'!C20</f>
         <v>3968</v>
       </c>
-      <c r="D26" s="53">
+      <c r="D26" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5537,11 +5588,11 @@
         <f>'Packet Rates'!J40*'Packet Sizes'!H20</f>
         <v>4648</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="15">
         <f>'Packet Rates'!K40*'Packet Sizes'!H20</f>
         <v>4648</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="17">
         <f t="shared" si="1"/>
         <v>31691</v>
       </c>
@@ -5549,7 +5600,7 @@
         <f t="shared" si="7"/>
         <v>49291</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="17">
         <f t="shared" si="3"/>
         <v>221837</v>
       </c>
@@ -5557,27 +5608,27 @@
         <f t="shared" si="4"/>
         <v>345037</v>
       </c>
-      <c r="P26" s="45">
+      <c r="P26" s="36">
         <f t="shared" si="5"/>
         <v>0.97302076203513577</v>
       </c>
-      <c r="Q26" s="46">
+      <c r="Q26" s="37">
         <f t="shared" si="6"/>
         <v>0.95803749902098001</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="26">
         <f>'Packet Rates'!C41*'Packet Sizes'!C21</f>
         <v>3968</v>
       </c>
-      <c r="D27" s="53">
+      <c r="D27" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5605,11 +5656,11 @@
         <f>'Packet Rates'!J41*'Packet Sizes'!H21</f>
         <v>4648</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="15">
         <f>'Packet Rates'!K41*'Packet Sizes'!H21</f>
         <v>4648</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="17">
         <f t="shared" si="1"/>
         <v>32971</v>
       </c>
@@ -5617,7 +5668,7 @@
         <f t="shared" si="7"/>
         <v>53131</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="17">
         <f t="shared" si="3"/>
         <v>230797</v>
       </c>
@@ -5625,27 +5676,27 @@
         <f t="shared" si="4"/>
         <v>371917</v>
       </c>
-      <c r="P27" s="45">
+      <c r="P27" s="36">
         <f t="shared" si="5"/>
         <v>0.97193107017956082</v>
       </c>
-      <c r="Q27" s="46">
+      <c r="Q27" s="37">
         <f t="shared" si="6"/>
         <v>0.95476842345425506</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="26">
         <f>'Packet Rates'!C42*'Packet Sizes'!C22</f>
         <v>3968</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5673,11 +5724,11 @@
         <f>'Packet Rates'!J42*'Packet Sizes'!H22</f>
         <v>4648</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="15">
         <f>'Packet Rates'!K42*'Packet Sizes'!H22</f>
         <v>4648</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="17">
         <f t="shared" si="1"/>
         <v>34829</v>
       </c>
@@ -5685,7 +5736,7 @@
         <f t="shared" si="7"/>
         <v>56269</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="17">
         <f t="shared" si="3"/>
         <v>243803</v>
       </c>
@@ -5693,27 +5744,27 @@
         <f t="shared" si="4"/>
         <v>393883</v>
       </c>
-      <c r="P28" s="45">
+      <c r="P28" s="36">
         <f t="shared" si="5"/>
         <v>0.9703493143454528</v>
       </c>
-      <c r="Q28" s="46">
+      <c r="Q28" s="37">
         <f t="shared" si="6"/>
         <v>0.95209697576457208</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="26">
         <f>'Packet Rates'!C43*'Packet Sizes'!C23</f>
         <v>3968</v>
       </c>
-      <c r="D29" s="53">
+      <c r="D29" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5741,11 +5792,11 @@
         <f>'Packet Rates'!J43*'Packet Sizes'!H23</f>
         <v>4648</v>
       </c>
-      <c r="K29" s="18">
+      <c r="K29" s="15">
         <f>'Packet Rates'!K43*'Packet Sizes'!H23</f>
         <v>4648</v>
       </c>
-      <c r="L29" s="20">
+      <c r="L29" s="17">
         <f t="shared" si="1"/>
         <v>34829</v>
       </c>
@@ -5753,7 +5804,7 @@
         <f t="shared" si="7"/>
         <v>56269</v>
       </c>
-      <c r="N29" s="20">
+      <c r="N29" s="17">
         <f t="shared" si="3"/>
         <v>243803</v>
       </c>
@@ -5761,27 +5812,27 @@
         <f t="shared" si="4"/>
         <v>393883</v>
       </c>
-      <c r="P29" s="45">
+      <c r="P29" s="36">
         <f t="shared" si="5"/>
         <v>0.9703493143454528</v>
       </c>
-      <c r="Q29" s="46">
+      <c r="Q29" s="37">
         <f t="shared" si="6"/>
         <v>0.95209697576457208</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="26">
         <f>'Packet Rates'!C44*'Packet Sizes'!C24</f>
         <v>3968</v>
       </c>
-      <c r="D30" s="53">
+      <c r="D30" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5809,11 +5860,11 @@
         <f>'Packet Rates'!J44*'Packet Sizes'!H24</f>
         <v>4648</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="15">
         <f>'Packet Rates'!K44*'Packet Sizes'!H24</f>
         <v>4648</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="17">
         <f t="shared" si="1"/>
         <v>34829</v>
       </c>
@@ -5821,7 +5872,7 @@
         <f t="shared" si="7"/>
         <v>56269</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="17">
         <f t="shared" si="3"/>
         <v>243803</v>
       </c>
@@ -5829,27 +5880,27 @@
         <f t="shared" si="4"/>
         <v>393883</v>
       </c>
-      <c r="P30" s="45">
+      <c r="P30" s="36">
         <f t="shared" si="5"/>
         <v>0.9703493143454528</v>
       </c>
-      <c r="Q30" s="46">
+      <c r="Q30" s="37">
         <f t="shared" si="6"/>
         <v>0.95209697576457208</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="26">
         <f>'Packet Rates'!C45*'Packet Sizes'!C25</f>
         <v>3968</v>
       </c>
-      <c r="D31" s="53">
+      <c r="D31" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5877,11 +5928,11 @@
         <f>'Packet Rates'!J45*'Packet Sizes'!H25</f>
         <v>4648</v>
       </c>
-      <c r="K31" s="18">
+      <c r="K31" s="15">
         <f>'Packet Rates'!K45*'Packet Sizes'!H25</f>
         <v>4648</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L31" s="17">
         <f t="shared" si="1"/>
         <v>35365</v>
       </c>
@@ -5889,7 +5940,7 @@
         <f t="shared" si="7"/>
         <v>56805</v>
       </c>
-      <c r="N31" s="20">
+      <c r="N31" s="17">
         <f t="shared" si="3"/>
         <v>247555</v>
       </c>
@@ -5897,27 +5948,27 @@
         <f t="shared" si="4"/>
         <v>397635</v>
       </c>
-      <c r="P31" s="45">
+      <c r="P31" s="36">
         <f t="shared" si="5"/>
         <v>0.96989300588093075</v>
       </c>
-      <c r="Q31" s="46">
+      <c r="Q31" s="37">
         <f t="shared" si="6"/>
         <v>0.95164066730005004</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="34">
+      <c r="C32" s="26">
         <f>'Packet Rates'!C46*'Packet Sizes'!C26</f>
         <v>3968</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D32" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5945,11 +5996,11 @@
         <f>'Packet Rates'!J46*'Packet Sizes'!H26</f>
         <v>4648</v>
       </c>
-      <c r="K32" s="18">
+      <c r="K32" s="15">
         <f>'Packet Rates'!K46*'Packet Sizes'!H26</f>
         <v>4648</v>
       </c>
-      <c r="L32" s="20">
+      <c r="L32" s="17">
         <f t="shared" si="1"/>
         <v>36273</v>
       </c>
@@ -5957,7 +6008,7 @@
         <f t="shared" si="7"/>
         <v>58993</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N32" s="17">
         <f t="shared" si="3"/>
         <v>253911</v>
       </c>
@@ -5965,27 +6016,27 @@
         <f t="shared" si="4"/>
         <v>412951</v>
       </c>
-      <c r="P32" s="45">
+      <c r="P32" s="36">
         <f t="shared" si="5"/>
         <v>0.96912000572088219</v>
       </c>
-      <c r="Q32" s="46">
+      <c r="Q32" s="37">
         <f t="shared" si="6"/>
         <v>0.94977797528442665</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="26">
         <f>'Packet Rates'!C47*'Packet Sizes'!C27</f>
         <v>3968</v>
       </c>
-      <c r="D33" s="53">
+      <c r="D33" s="44">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -6013,11 +6064,11 @@
         <f>'Packet Rates'!J47*'Packet Sizes'!H27</f>
         <v>4648</v>
       </c>
-      <c r="K33" s="18">
+      <c r="K33" s="15">
         <f>'Packet Rates'!K47*'Packet Sizes'!H27</f>
         <v>4648</v>
       </c>
-      <c r="L33" s="20">
+      <c r="L33" s="17">
         <f t="shared" si="1"/>
         <v>36913</v>
       </c>
@@ -6025,7 +6076,7 @@
         <f t="shared" si="7"/>
         <v>60913</v>
       </c>
-      <c r="N33" s="20">
+      <c r="N33" s="17">
         <f t="shared" si="3"/>
         <v>258391</v>
       </c>
@@ -6033,27 +6084,27 @@
         <f t="shared" si="4"/>
         <v>426391</v>
       </c>
-      <c r="P33" s="45">
+      <c r="P33" s="36">
         <f t="shared" si="5"/>
         <v>0.96857515979309472</v>
       </c>
-      <c r="Q33" s="46">
+      <c r="Q33" s="37">
         <f t="shared" si="6"/>
         <v>0.94814343750106411</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="26">
         <f>'Packet Rates'!C48*'Packet Sizes'!C28</f>
         <v>3968</v>
       </c>
-      <c r="D34" s="53">
+      <c r="D34" s="44">
         <f t="shared" ref="D34:D37" si="8">1-(C34/$C$18)</f>
         <v>0.96915422885572144</v>
       </c>
@@ -6081,11 +6132,11 @@
         <f>'Packet Rates'!J48*'Packet Sizes'!H28</f>
         <v>3752</v>
       </c>
-      <c r="K34" s="18">
+      <c r="K34" s="15">
         <f>'Packet Rates'!K48*'Packet Sizes'!H28</f>
         <v>3752</v>
       </c>
-      <c r="L34" s="20">
+      <c r="L34" s="17">
         <f t="shared" ref="L34:L37" si="9">E34+G34+H34+I34+J34</f>
         <v>36017</v>
       </c>
@@ -6093,7 +6144,7 @@
         <f t="shared" ref="M34:M37" si="10">F34+G34+H34+I34+K34</f>
         <v>60017</v>
       </c>
-      <c r="N34" s="20">
+      <c r="N34" s="17">
         <f t="shared" ref="N34:N37" si="11">L34*7</f>
         <v>252119</v>
       </c>
@@ -6101,27 +6152,27 @@
         <f t="shared" ref="O34:O37" si="12">M34*7</f>
         <v>420119</v>
       </c>
-      <c r="P34" s="45">
+      <c r="P34" s="36">
         <f t="shared" ref="P34:P37" si="13">1-(N34/$N$18)</f>
         <v>0.96933794409199725</v>
       </c>
-      <c r="Q34" s="46">
+      <c r="Q34" s="37">
         <f t="shared" ref="Q34:Q37" si="14">1-(O34/$O$18)</f>
         <v>0.94890622179996664</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="26">
         <f>'Packet Rates'!C49*'Packet Sizes'!C29</f>
         <v>3968</v>
       </c>
-      <c r="D35" s="53">
+      <c r="D35" s="44">
         <f t="shared" si="8"/>
         <v>0.96915422885572144</v>
       </c>
@@ -6149,11 +6200,11 @@
         <f>'Packet Rates'!J49*'Packet Sizes'!H29</f>
         <v>3752</v>
       </c>
-      <c r="K35" s="18">
+      <c r="K35" s="15">
         <f>'Packet Rates'!K49*'Packet Sizes'!H29</f>
         <v>3752</v>
       </c>
-      <c r="L35" s="20">
+      <c r="L35" s="17">
         <f t="shared" si="9"/>
         <v>36017</v>
       </c>
@@ -6161,7 +6212,7 @@
         <f t="shared" si="10"/>
         <v>60017</v>
       </c>
-      <c r="N35" s="20">
+      <c r="N35" s="17">
         <f t="shared" si="11"/>
         <v>252119</v>
       </c>
@@ -6169,27 +6220,27 @@
         <f t="shared" si="12"/>
         <v>420119</v>
       </c>
-      <c r="P35" s="45">
+      <c r="P35" s="36">
         <f t="shared" si="13"/>
         <v>0.96933794409199725</v>
       </c>
-      <c r="Q35" s="46">
+      <c r="Q35" s="37">
         <f t="shared" si="14"/>
         <v>0.94890622179996664</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="34">
+      <c r="C36" s="26">
         <f>'Packet Rates'!C50*'Packet Sizes'!C30</f>
         <v>3968</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D36" s="44">
         <f t="shared" si="8"/>
         <v>0.96915422885572144</v>
       </c>
@@ -6217,11 +6268,11 @@
         <f>'Packet Rates'!J50*'Packet Sizes'!H30</f>
         <v>3752</v>
       </c>
-      <c r="K36" s="18">
+      <c r="K36" s="15">
         <f>'Packet Rates'!K50*'Packet Sizes'!H30</f>
         <v>3752</v>
       </c>
-      <c r="L36" s="20">
+      <c r="L36" s="17">
         <f t="shared" si="9"/>
         <v>36017</v>
       </c>
@@ -6229,7 +6280,7 @@
         <f t="shared" si="10"/>
         <v>60017</v>
       </c>
-      <c r="N36" s="20">
+      <c r="N36" s="17">
         <f t="shared" si="11"/>
         <v>252119</v>
       </c>
@@ -6237,27 +6288,27 @@
         <f t="shared" si="12"/>
         <v>420119</v>
       </c>
-      <c r="P36" s="45">
+      <c r="P36" s="36">
         <f t="shared" si="13"/>
         <v>0.96933794409199725</v>
       </c>
-      <c r="Q36" s="46">
+      <c r="Q36" s="37">
         <f t="shared" si="14"/>
         <v>0.94890622179996664</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C37" s="26">
         <f>'Packet Rates'!C51*'Packet Sizes'!C31</f>
         <v>3968</v>
       </c>
-      <c r="D37" s="53">
+      <c r="D37" s="44">
         <f t="shared" si="8"/>
         <v>0.96915422885572144</v>
       </c>
@@ -6285,11 +6336,11 @@
         <f>'Packet Rates'!J51*'Packet Sizes'!H31</f>
         <v>3752</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="15">
         <f>'Packet Rates'!K51*'Packet Sizes'!H31</f>
         <v>3752</v>
       </c>
-      <c r="L37" s="20">
+      <c r="L37" s="17">
         <f t="shared" si="9"/>
         <v>37937</v>
       </c>
@@ -6297,7 +6348,7 @@
         <f t="shared" si="10"/>
         <v>65777</v>
       </c>
-      <c r="N37" s="20">
+      <c r="N37" s="17">
         <f t="shared" si="11"/>
         <v>265559</v>
       </c>
@@ -6305,27 +6356,27 @@
         <f t="shared" si="12"/>
         <v>460439</v>
       </c>
-      <c r="P37" s="45">
+      <c r="P37" s="36">
         <f t="shared" si="13"/>
         <v>0.96770340630863483</v>
       </c>
-      <c r="Q37" s="46">
+      <c r="Q37" s="37">
         <f t="shared" si="14"/>
         <v>0.94400260844987927</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="26">
         <f>'Packet Rates'!C52*'Packet Sizes'!C32</f>
         <v>3968</v>
       </c>
-      <c r="D38" s="53">
+      <c r="D38" s="44">
         <f t="shared" ref="D38" si="15">1-(C38/$C$18)</f>
         <v>0.96915422885572144</v>
       </c>
@@ -6353,11 +6404,11 @@
         <f>'Packet Rates'!J52*'Packet Sizes'!H32</f>
         <v>10720</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="15">
         <f>'Packet Rates'!K52*'Packet Sizes'!H32</f>
         <v>10720</v>
       </c>
-      <c r="L38" s="20">
+      <c r="L38" s="17">
         <f t="shared" ref="L38" si="16">E38+G38+H38+I38+J38</f>
         <v>44905</v>
       </c>
@@ -6365,7 +6416,7 @@
         <f t="shared" ref="M38" si="17">F38+G38+H38+I38+K38</f>
         <v>72745</v>
       </c>
-      <c r="N38" s="20">
+      <c r="N38" s="17">
         <f t="shared" ref="N38" si="18">L38*7</f>
         <v>314335</v>
       </c>
@@ -6373,36 +6424,94 @@
         <f t="shared" ref="O38" si="19">M38*7</f>
         <v>509215</v>
       </c>
-      <c r="P38" s="45">
+      <c r="P38" s="36">
         <f t="shared" ref="P38" si="20">1-(N38/$N$18)</f>
         <v>0.96177139626984853</v>
       </c>
-      <c r="Q38" s="46">
+      <c r="Q38" s="37">
         <f t="shared" ref="Q38" si="21">1-(O38/$O$18)</f>
         <v>0.93807059841109308</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="46"/>
+      <c r="A39" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="26">
+        <f>'Packet Rates'!C53*'Packet Sizes'!C33</f>
+        <v>4480</v>
+      </c>
+      <c r="D39" s="44">
+        <f t="shared" ref="D39" si="22">1-(C39/$C$18)</f>
+        <v>0.96517412935323388</v>
+      </c>
+      <c r="E39" s="9">
+        <f>'Packet Rates'!E53*'Packet Sizes'!D33</f>
+        <v>14560</v>
+      </c>
+      <c r="F39" s="10">
+        <f>'Packet Rates'!F53*'Packet Sizes'!D33</f>
+        <v>43680</v>
+      </c>
+      <c r="G39" s="10">
+        <f>'Packet Rates'!G53*'Packet Sizes'!E33</f>
+        <v>11040</v>
+      </c>
+      <c r="H39" s="10">
+        <f>'Packet Rates'!H53*'Packet Sizes'!F33</f>
+        <v>6901</v>
+      </c>
+      <c r="I39" s="10">
+        <f>'Packet Rates'!I53*'Packet Sizes'!G33</f>
+        <v>2324</v>
+      </c>
+      <c r="J39" s="10">
+        <f>'Packet Rates'!J53*'Packet Sizes'!H33</f>
+        <v>10720</v>
+      </c>
+      <c r="K39" s="15">
+        <f>'Packet Rates'!K53*'Packet Sizes'!H33</f>
+        <v>10720</v>
+      </c>
+      <c r="L39" s="17">
+        <f t="shared" ref="L39" si="23">E39+G39+H39+I39+J39</f>
+        <v>45545</v>
+      </c>
+      <c r="M39" s="11">
+        <f t="shared" ref="M39" si="24">F39+G39+H39+I39+K39</f>
+        <v>74665</v>
+      </c>
+      <c r="N39" s="17">
+        <f t="shared" ref="N39" si="25">L39*7</f>
+        <v>318815</v>
+      </c>
+      <c r="O39" s="11">
+        <f t="shared" ref="O39" si="26">M39*7</f>
+        <v>522655</v>
+      </c>
+      <c r="P39" s="36">
+        <f t="shared" ref="P39" si="27">1-(N39/$N$18)</f>
+        <v>0.96122655034206106</v>
+      </c>
+      <c r="Q39" s="37">
+        <f t="shared" ref="Q39" si="28">1-(O39/$O$18)</f>
+        <v>0.93643606062773066</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="E15:M15"/>
@@ -6417,16 +6526,8 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C18:D39">
     <cfRule type="colorScale" priority="17">
       <colorScale>
@@ -6535,7 +6636,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P38">
+  <conditionalFormatting sqref="P18:P39">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6599,7 +6700,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18:Q38">
+  <conditionalFormatting sqref="Q18:Q39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>